<commit_message>
Preparing new version of data, and starting building new model.
</commit_message>
<xml_diff>
--- a/Settings/SA_setting.xlsx
+++ b/Settings/SA_setting.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\nauka\GitHub\cge_model_python\Data\Raw data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\nauka\GitHub\cge_model_python\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216941BA-D7CF-42CA-A145-0908D4FAF2D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93C9A93-0D2D-4001-83A1-7EA3BD66F6DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -608,25 +608,25 @@
     <t/>
   </si>
   <si>
-    <t>taxes</t>
-  </si>
-  <si>
-    <t>atax</t>
-  </si>
-  <si>
     <t>dtax</t>
   </si>
   <si>
-    <t>mtax</t>
-  </si>
-  <si>
     <t>stax</t>
   </si>
   <si>
-    <t>goods_production</t>
-  </si>
-  <si>
-    <t>goods_consumption</t>
+    <t>government</t>
+  </si>
+  <si>
+    <t>goods_activities</t>
+  </si>
+  <si>
+    <t>goods_commodities</t>
+  </si>
+  <si>
+    <t>inc_taxes</t>
+  </si>
+  <si>
+    <t>cons_taxes</t>
   </si>
 </sst>
 </file>
@@ -944,23 +944,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E105"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>166</v>
       </c>
       <c r="B1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" t="s">
         <v>182</v>
-      </c>
-      <c r="C1" t="s">
-        <v>189</v>
       </c>
       <c r="D1" t="s">
         <v>194</v>
@@ -968,845 +968,845 @@
       <c r="E1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>167</v>
       </c>
       <c r="B2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" t="s">
         <v>183</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" t="s">
         <v>190</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>168</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>184</v>
       </c>
-      <c r="C3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>169</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>185</v>
       </c>
-      <c r="C4" t="s">
-        <v>192</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>170</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>186</v>
       </c>
-      <c r="C5" t="s">
-        <v>193</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>171</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>187</v>
       </c>
-      <c r="C6" t="s">
-        <v>188</v>
-      </c>
       <c r="D6" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>172</v>
       </c>
-      <c r="B7" t="s">
-        <v>188</v>
-      </c>
       <c r="C7" t="s">
         <v>188</v>
       </c>
       <c r="D7" t="s">
+        <v>188</v>
+      </c>
+      <c r="F7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>173</v>
       </c>
-      <c r="B8" t="s">
-        <v>188</v>
-      </c>
       <c r="C8" t="s">
         <v>188</v>
       </c>
       <c r="D8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>174</v>
       </c>
-      <c r="B9" t="s">
-        <v>188</v>
-      </c>
       <c r="C9" t="s">
         <v>188</v>
       </c>
       <c r="D9" t="s">
+        <v>188</v>
+      </c>
+      <c r="F9" t="s">
         <v>7</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>175</v>
       </c>
-      <c r="B10" t="s">
-        <v>188</v>
-      </c>
       <c r="C10" t="s">
         <v>188</v>
       </c>
       <c r="D10" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>176</v>
       </c>
-      <c r="B11" t="s">
-        <v>188</v>
-      </c>
       <c r="C11" t="s">
         <v>188</v>
       </c>
       <c r="D11" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" t="s">
         <v>9</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>177</v>
       </c>
-      <c r="B12" t="s">
-        <v>188</v>
-      </c>
       <c r="C12" t="s">
         <v>188</v>
       </c>
       <c r="D12" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" t="s">
         <v>10</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>178</v>
       </c>
-      <c r="B13" t="s">
-        <v>188</v>
-      </c>
       <c r="C13" t="s">
         <v>188</v>
       </c>
       <c r="D13" t="s">
+        <v>188</v>
+      </c>
+      <c r="F13" t="s">
         <v>11</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>179</v>
       </c>
-      <c r="B14" t="s">
-        <v>188</v>
-      </c>
       <c r="C14" t="s">
         <v>188</v>
       </c>
       <c r="D14" t="s">
+        <v>188</v>
+      </c>
+      <c r="F14" t="s">
         <v>12</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>180</v>
       </c>
-      <c r="B15" t="s">
-        <v>188</v>
-      </c>
       <c r="C15" t="s">
         <v>188</v>
       </c>
       <c r="D15" t="s">
+        <v>188</v>
+      </c>
+      <c r="F15" t="s">
         <v>13</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>181</v>
-      </c>
-      <c r="B16" t="s">
-        <v>188</v>
-      </c>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>188</v>
       </c>
       <c r="D16" t="s">
+        <v>188</v>
+      </c>
+      <c r="F16" t="s">
         <v>14</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
         <v>15</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
         <v>16</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
         <v>17</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
+    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
         <v>18</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
         <v>19</v>
       </c>
-      <c r="E21" t="s">
+      <c r="G21" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
+    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
         <v>20</v>
       </c>
-      <c r="E22" t="s">
+      <c r="G22" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
         <v>21</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
+    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
         <v>22</v>
       </c>
-      <c r="E24" t="s">
+      <c r="G24" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
+    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
         <v>23</v>
       </c>
-      <c r="E25" t="s">
+      <c r="G25" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
+    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
         <v>24</v>
       </c>
-      <c r="E26" t="s">
+      <c r="G26" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
+    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
         <v>25</v>
       </c>
-      <c r="E27" t="s">
+      <c r="G27" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
+    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
         <v>26</v>
       </c>
-      <c r="E28" t="s">
+      <c r="G28" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
+    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
         <v>27</v>
       </c>
-      <c r="E29" t="s">
+      <c r="G29" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
+    <row r="30" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
         <v>28</v>
       </c>
-      <c r="E30" t="s">
+      <c r="G30" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
+    <row r="31" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
         <v>29</v>
       </c>
-      <c r="E31" t="s">
+      <c r="G31" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
+    <row r="32" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
         <v>30</v>
       </c>
-      <c r="E32" t="s">
+      <c r="G32" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
         <v>31</v>
       </c>
-      <c r="E33" t="s">
+      <c r="G33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
         <v>32</v>
       </c>
-      <c r="E34" t="s">
+      <c r="G34" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
         <v>33</v>
       </c>
-      <c r="E35" t="s">
+      <c r="G35" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
         <v>34</v>
       </c>
-      <c r="E36" t="s">
+      <c r="G36" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
+    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
         <v>35</v>
       </c>
-      <c r="E37" t="s">
+      <c r="G37" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
+    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
         <v>36</v>
       </c>
-      <c r="E38" t="s">
+      <c r="G38" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
         <v>37</v>
       </c>
-      <c r="E39" t="s">
+      <c r="G39" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
+    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
         <v>38</v>
       </c>
-      <c r="E40" t="s">
+      <c r="G40" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D41" t="s">
+    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
         <v>39</v>
       </c>
-      <c r="E41" t="s">
+      <c r="G41" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
+    <row r="42" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
         <v>40</v>
       </c>
-      <c r="E42" t="s">
+      <c r="G42" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
+    <row r="43" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
         <v>41</v>
       </c>
-      <c r="E43" t="s">
+      <c r="G43" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
+    <row r="44" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
         <v>42</v>
       </c>
-      <c r="E44" t="s">
+      <c r="G44" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D45" t="s">
+    <row r="45" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
         <v>43</v>
       </c>
-      <c r="E45" t="s">
+      <c r="G45" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D46" t="s">
+    <row r="46" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
         <v>44</v>
       </c>
-      <c r="E46" t="s">
+      <c r="G46" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D47" t="s">
+    <row r="47" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
         <v>45</v>
       </c>
-      <c r="E47" t="s">
+      <c r="G47" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D48" t="s">
+    <row r="48" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
         <v>46</v>
       </c>
-      <c r="E48" t="s">
+      <c r="G48" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D49" t="s">
+    <row r="49" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
         <v>47</v>
       </c>
-      <c r="E49" t="s">
+      <c r="G49" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D50" t="s">
+    <row r="50" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
         <v>48</v>
       </c>
-      <c r="E50" t="s">
+      <c r="G50" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
+    <row r="51" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
         <v>49</v>
       </c>
-      <c r="E51" t="s">
+      <c r="G51" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D52" t="s">
+    <row r="52" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
         <v>50</v>
       </c>
-      <c r="E52" t="s">
+      <c r="G52" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D53" t="s">
+    <row r="53" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
         <v>51</v>
       </c>
-      <c r="E53" t="s">
+      <c r="G53" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D54" t="s">
+    <row r="54" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
         <v>52</v>
       </c>
-      <c r="E54" t="s">
+      <c r="G54" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D55" t="s">
+    <row r="55" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
         <v>53</v>
       </c>
-      <c r="E55" t="s">
+      <c r="G55" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D56" t="s">
+    <row r="56" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
         <v>54</v>
       </c>
-      <c r="E56" t="s">
+      <c r="G56" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D57" t="s">
+    <row r="57" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
         <v>55</v>
       </c>
-      <c r="E57" t="s">
+      <c r="G57" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
+    <row r="58" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
         <v>56</v>
       </c>
-      <c r="E58" t="s">
+      <c r="G58" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="59" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
+    <row r="59" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
         <v>57</v>
       </c>
-      <c r="E59" t="s">
+      <c r="G59" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="60" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
+    <row r="60" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
         <v>58</v>
       </c>
-      <c r="E60" t="s">
+      <c r="G60" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
+    <row r="61" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F61" t="s">
         <v>59</v>
       </c>
-      <c r="E61" t="s">
+      <c r="G61" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="62" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D62" t="s">
+    <row r="62" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F62" t="s">
         <v>60</v>
       </c>
-      <c r="E62" t="s">
+      <c r="G62" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="63" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D63" t="s">
+    <row r="63" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F63" t="s">
         <v>61</v>
       </c>
-      <c r="E63" t="s">
+      <c r="G63" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E64" t="s">
+    <row r="64" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G64" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E65" t="s">
+    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G65" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E66" t="s">
+    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G66" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E67" t="s">
+    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G67" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E68" t="s">
+    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G68" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E69" t="s">
+    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G69" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E70" t="s">
+    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G70" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E71" t="s">
+    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G71" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E72" t="s">
+    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G72" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E73" t="s">
+    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G73" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E74" t="s">
+    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E75" t="s">
+    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E76" t="s">
+    <row r="76" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G76" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E77" t="s">
+    <row r="77" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G77" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E78" t="s">
+    <row r="78" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G78" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E79" t="s">
+    <row r="79" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G79" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E80" t="s">
+    <row r="80" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G80" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E81" t="s">
+    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G81" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E82" t="s">
+    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G82" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E83" t="s">
+    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G83" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E84" t="s">
+    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G84" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E85" t="s">
+    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G85" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E86" t="s">
+    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G86" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E87" t="s">
+    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G87" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E88" t="s">
+    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G88" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E89" t="s">
+    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G89" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E90" t="s">
+    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G90" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E91" t="s">
+    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G91" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E92" t="s">
+    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G92" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E93" t="s">
+    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G93" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E94" t="s">
+    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G94" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E95" t="s">
+    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G95" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E96" t="s">
+    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G96" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E97" t="s">
+    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G97" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E98" t="s">
+    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G98" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E99" t="s">
+    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G99" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E100" t="s">
+    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G100" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E101" t="s">
+    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G101" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E102" t="s">
+    <row r="102" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G102" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E103" t="s">
+    <row r="103" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G103" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E104" t="s">
+    <row r="104" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G104" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E105" t="s">
+    <row r="105" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G105" t="s">
         <v>165</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding new SAM data.
</commit_message>
<xml_diff>
--- a/Settings/SA_setting.xlsx
+++ b/Settings/SA_setting.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\nauka\GitHub\cge_model_python\Data\Raw data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\nauka\GitHub\cge_model_python\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216941BA-D7CF-42CA-A145-0908D4FAF2D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93C9A93-0D2D-4001-83A1-7EA3BD66F6DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -608,25 +608,25 @@
     <t/>
   </si>
   <si>
-    <t>taxes</t>
-  </si>
-  <si>
-    <t>atax</t>
-  </si>
-  <si>
     <t>dtax</t>
   </si>
   <si>
-    <t>mtax</t>
-  </si>
-  <si>
     <t>stax</t>
   </si>
   <si>
-    <t>goods_production</t>
-  </si>
-  <si>
-    <t>goods_consumption</t>
+    <t>government</t>
+  </si>
+  <si>
+    <t>goods_activities</t>
+  </si>
+  <si>
+    <t>goods_commodities</t>
+  </si>
+  <si>
+    <t>inc_taxes</t>
+  </si>
+  <si>
+    <t>cons_taxes</t>
   </si>
 </sst>
 </file>
@@ -944,23 +944,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E105"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>166</v>
       </c>
       <c r="B1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" t="s">
         <v>182</v>
-      </c>
-      <c r="C1" t="s">
-        <v>189</v>
       </c>
       <c r="D1" t="s">
         <v>194</v>
@@ -968,845 +968,845 @@
       <c r="E1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>167</v>
       </c>
       <c r="B2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" t="s">
         <v>183</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" t="s">
         <v>190</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>168</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>184</v>
       </c>
-      <c r="C3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>169</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>185</v>
       </c>
-      <c r="C4" t="s">
-        <v>192</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>170</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>186</v>
       </c>
-      <c r="C5" t="s">
-        <v>193</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>171</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>187</v>
       </c>
-      <c r="C6" t="s">
-        <v>188</v>
-      </c>
       <c r="D6" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>172</v>
       </c>
-      <c r="B7" t="s">
-        <v>188</v>
-      </c>
       <c r="C7" t="s">
         <v>188</v>
       </c>
       <c r="D7" t="s">
+        <v>188</v>
+      </c>
+      <c r="F7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>173</v>
       </c>
-      <c r="B8" t="s">
-        <v>188</v>
-      </c>
       <c r="C8" t="s">
         <v>188</v>
       </c>
       <c r="D8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>174</v>
       </c>
-      <c r="B9" t="s">
-        <v>188</v>
-      </c>
       <c r="C9" t="s">
         <v>188</v>
       </c>
       <c r="D9" t="s">
+        <v>188</v>
+      </c>
+      <c r="F9" t="s">
         <v>7</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>175</v>
       </c>
-      <c r="B10" t="s">
-        <v>188</v>
-      </c>
       <c r="C10" t="s">
         <v>188</v>
       </c>
       <c r="D10" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>176</v>
       </c>
-      <c r="B11" t="s">
-        <v>188</v>
-      </c>
       <c r="C11" t="s">
         <v>188</v>
       </c>
       <c r="D11" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" t="s">
         <v>9</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>177</v>
       </c>
-      <c r="B12" t="s">
-        <v>188</v>
-      </c>
       <c r="C12" t="s">
         <v>188</v>
       </c>
       <c r="D12" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" t="s">
         <v>10</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>178</v>
       </c>
-      <c r="B13" t="s">
-        <v>188</v>
-      </c>
       <c r="C13" t="s">
         <v>188</v>
       </c>
       <c r="D13" t="s">
+        <v>188</v>
+      </c>
+      <c r="F13" t="s">
         <v>11</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>179</v>
       </c>
-      <c r="B14" t="s">
-        <v>188</v>
-      </c>
       <c r="C14" t="s">
         <v>188</v>
       </c>
       <c r="D14" t="s">
+        <v>188</v>
+      </c>
+      <c r="F14" t="s">
         <v>12</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>180</v>
       </c>
-      <c r="B15" t="s">
-        <v>188</v>
-      </c>
       <c r="C15" t="s">
         <v>188</v>
       </c>
       <c r="D15" t="s">
+        <v>188</v>
+      </c>
+      <c r="F15" t="s">
         <v>13</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>181</v>
-      </c>
-      <c r="B16" t="s">
-        <v>188</v>
-      </c>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>188</v>
       </c>
       <c r="D16" t="s">
+        <v>188</v>
+      </c>
+      <c r="F16" t="s">
         <v>14</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
         <v>15</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
         <v>16</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
         <v>17</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
+    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
         <v>18</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
         <v>19</v>
       </c>
-      <c r="E21" t="s">
+      <c r="G21" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
+    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
         <v>20</v>
       </c>
-      <c r="E22" t="s">
+      <c r="G22" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
         <v>21</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
+    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
         <v>22</v>
       </c>
-      <c r="E24" t="s">
+      <c r="G24" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
+    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
         <v>23</v>
       </c>
-      <c r="E25" t="s">
+      <c r="G25" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
+    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
         <v>24</v>
       </c>
-      <c r="E26" t="s">
+      <c r="G26" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
+    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
         <v>25</v>
       </c>
-      <c r="E27" t="s">
+      <c r="G27" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
+    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
         <v>26</v>
       </c>
-      <c r="E28" t="s">
+      <c r="G28" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
+    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
         <v>27</v>
       </c>
-      <c r="E29" t="s">
+      <c r="G29" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
+    <row r="30" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
         <v>28</v>
       </c>
-      <c r="E30" t="s">
+      <c r="G30" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
+    <row r="31" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
         <v>29</v>
       </c>
-      <c r="E31" t="s">
+      <c r="G31" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
+    <row r="32" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
         <v>30</v>
       </c>
-      <c r="E32" t="s">
+      <c r="G32" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
         <v>31</v>
       </c>
-      <c r="E33" t="s">
+      <c r="G33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
         <v>32</v>
       </c>
-      <c r="E34" t="s">
+      <c r="G34" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
         <v>33</v>
       </c>
-      <c r="E35" t="s">
+      <c r="G35" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
         <v>34</v>
       </c>
-      <c r="E36" t="s">
+      <c r="G36" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
+    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
         <v>35</v>
       </c>
-      <c r="E37" t="s">
+      <c r="G37" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
+    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
         <v>36</v>
       </c>
-      <c r="E38" t="s">
+      <c r="G38" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
         <v>37</v>
       </c>
-      <c r="E39" t="s">
+      <c r="G39" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
+    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
         <v>38</v>
       </c>
-      <c r="E40" t="s">
+      <c r="G40" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D41" t="s">
+    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
         <v>39</v>
       </c>
-      <c r="E41" t="s">
+      <c r="G41" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
+    <row r="42" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
         <v>40</v>
       </c>
-      <c r="E42" t="s">
+      <c r="G42" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
+    <row r="43" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
         <v>41</v>
       </c>
-      <c r="E43" t="s">
+      <c r="G43" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
+    <row r="44" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
         <v>42</v>
       </c>
-      <c r="E44" t="s">
+      <c r="G44" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D45" t="s">
+    <row r="45" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
         <v>43</v>
       </c>
-      <c r="E45" t="s">
+      <c r="G45" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D46" t="s">
+    <row r="46" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
         <v>44</v>
       </c>
-      <c r="E46" t="s">
+      <c r="G46" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D47" t="s">
+    <row r="47" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
         <v>45</v>
       </c>
-      <c r="E47" t="s">
+      <c r="G47" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D48" t="s">
+    <row r="48" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
         <v>46</v>
       </c>
-      <c r="E48" t="s">
+      <c r="G48" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D49" t="s">
+    <row r="49" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
         <v>47</v>
       </c>
-      <c r="E49" t="s">
+      <c r="G49" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D50" t="s">
+    <row r="50" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
         <v>48</v>
       </c>
-      <c r="E50" t="s">
+      <c r="G50" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
+    <row r="51" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
         <v>49</v>
       </c>
-      <c r="E51" t="s">
+      <c r="G51" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D52" t="s">
+    <row r="52" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
         <v>50</v>
       </c>
-      <c r="E52" t="s">
+      <c r="G52" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D53" t="s">
+    <row r="53" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
         <v>51</v>
       </c>
-      <c r="E53" t="s">
+      <c r="G53" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D54" t="s">
+    <row r="54" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
         <v>52</v>
       </c>
-      <c r="E54" t="s">
+      <c r="G54" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D55" t="s">
+    <row r="55" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
         <v>53</v>
       </c>
-      <c r="E55" t="s">
+      <c r="G55" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D56" t="s">
+    <row r="56" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
         <v>54</v>
       </c>
-      <c r="E56" t="s">
+      <c r="G56" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D57" t="s">
+    <row r="57" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
         <v>55</v>
       </c>
-      <c r="E57" t="s">
+      <c r="G57" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
+    <row r="58" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
         <v>56</v>
       </c>
-      <c r="E58" t="s">
+      <c r="G58" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="59" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
+    <row r="59" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
         <v>57</v>
       </c>
-      <c r="E59" t="s">
+      <c r="G59" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="60" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
+    <row r="60" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
         <v>58</v>
       </c>
-      <c r="E60" t="s">
+      <c r="G60" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
+    <row r="61" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F61" t="s">
         <v>59</v>
       </c>
-      <c r="E61" t="s">
+      <c r="G61" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="62" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D62" t="s">
+    <row r="62" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F62" t="s">
         <v>60</v>
       </c>
-      <c r="E62" t="s">
+      <c r="G62" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="63" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D63" t="s">
+    <row r="63" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F63" t="s">
         <v>61</v>
       </c>
-      <c r="E63" t="s">
+      <c r="G63" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E64" t="s">
+    <row r="64" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G64" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E65" t="s">
+    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G65" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E66" t="s">
+    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G66" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E67" t="s">
+    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G67" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E68" t="s">
+    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G68" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E69" t="s">
+    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G69" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E70" t="s">
+    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G70" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E71" t="s">
+    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G71" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E72" t="s">
+    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G72" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E73" t="s">
+    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G73" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E74" t="s">
+    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E75" t="s">
+    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E76" t="s">
+    <row r="76" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G76" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E77" t="s">
+    <row r="77" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G77" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E78" t="s">
+    <row r="78" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G78" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E79" t="s">
+    <row r="79" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G79" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E80" t="s">
+    <row r="80" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G80" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E81" t="s">
+    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G81" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E82" t="s">
+    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G82" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E83" t="s">
+    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G83" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E84" t="s">
+    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G84" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E85" t="s">
+    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G85" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E86" t="s">
+    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G86" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E87" t="s">
+    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G87" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E88" t="s">
+    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G88" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E89" t="s">
+    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G89" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E90" t="s">
+    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G90" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E91" t="s">
+    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G91" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E92" t="s">
+    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G92" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E93" t="s">
+    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G93" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E94" t="s">
+    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G94" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E95" t="s">
+    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G95" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E96" t="s">
+    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G96" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E97" t="s">
+    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G97" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E98" t="s">
+    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G98" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E99" t="s">
+    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G99" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E100" t="s">
+    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G100" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E101" t="s">
+    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G101" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E102" t="s">
+    <row r="102" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G102" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E103" t="s">
+    <row r="103" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G103" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E104" t="s">
+    <row r="104" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G104" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E105" t="s">
+    <row r="105" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G105" t="s">
         <v>165</v>
       </c>
     </row>

</xml_diff>